<commit_message>
update excel sheet with false biolog
</commit_message>
<xml_diff>
--- a/data/BIOLOG/Biolog21/211203_PM-BiologGSMMComp035.xlsx
+++ b/data/BIOLOG/Biolog21/211203_PM-BiologGSMMComp035.xlsx
@@ -1762,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1824,6 +1824,12 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
       <c r="I2">
         <v>1</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" t="e">
         <f>#N/A</f>
@@ -2127,7 +2133,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B13" t="s">
@@ -2139,11 +2145,11 @@
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="4">
-        <v>0.48</v>
+      <c r="E13">
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -2172,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -2188,7 +2194,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B15" t="s">
@@ -2200,11 +2206,11 @@
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="4">
-        <v>0.48</v>
+      <c r="E15">
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -2285,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G18" t="e">
         <f>#N/A</f>
@@ -2331,7 +2337,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B20" t="s">
@@ -2343,11 +2349,11 @@
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="4">
-        <v>0.24</v>
+      <c r="E20">
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2505,7 +2511,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B26" t="s">
@@ -2517,11 +2523,11 @@
       <c r="D26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="4">
-        <v>0.48</v>
+      <c r="E26">
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -2547,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2637,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2778,7 +2784,7 @@
       <c r="D35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35">
         <v>0.96</v>
       </c>
       <c r="F35">
@@ -2795,7 +2801,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B36" t="s">
@@ -2807,11 +2813,11 @@
       <c r="D36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="4">
-        <v>0.96</v>
+      <c r="E36">
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2840,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2933,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -2962,10 +2968,10 @@
         <v>11</v>
       </c>
       <c r="E41">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G41">
         <v>0.246992190847902</v>
@@ -2991,7 +2997,7 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3019,7 +3025,7 @@
       <c r="D43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43">
         <v>0.05</v>
       </c>
       <c r="F43">
@@ -3082,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3269,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -3285,7 +3291,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B52" t="s">
@@ -3298,10 +3304,10 @@
         <v>11</v>
       </c>
       <c r="E52">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G52">
         <v>0.493984381695804</v>
@@ -3330,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -3359,7 +3365,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -3388,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3420,7 +3426,7 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -3471,7 +3477,7 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B58" t="s">
@@ -3484,10 +3490,10 @@
         <v>11</v>
       </c>
       <c r="E58">
-        <v>0.43</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G58">
         <v>0.45787218735983198</v>
@@ -3691,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3755,7 +3761,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3816,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -3874,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3890,7 +3896,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B72" t="s">
@@ -3903,10 +3909,10 @@
         <v>11</v>
       </c>
       <c r="E72">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G72">
         <v>0.987968763391607</v>
@@ -3980,7 +3986,7 @@
       </c>
     </row>
     <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B75" t="s">
@@ -3996,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4079,7 +4085,7 @@
       <c r="D78" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78">
         <v>0.09</v>
       </c>
       <c r="F78">
@@ -4122,7 +4128,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B80" t="s">
@@ -4135,10 +4141,10 @@
         <v>11</v>
       </c>
       <c r="E80">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G80">
         <v>0.144501967466519</v>
@@ -4167,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -4337,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -4369,7 +4375,7 @@
         <v>0</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4430,7 +4436,7 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -4462,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4497,7 +4503,7 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4526,10 +4532,10 @@
         <v>11</v>
       </c>
       <c r="E93">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G93">
         <v>8.6928549643656094E-2</v>
@@ -4561,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4603,7 +4609,7 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="2" t="s">
         <v>273</v>
       </c>
       <c r="B96" t="s">
@@ -4615,11 +4621,11 @@
       <c r="D96" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E96" s="4">
-        <v>0.43</v>
+      <c r="E96">
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4673,8 +4679,11 @@
       <c r="D98" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
       <c r="F98">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G98" t="e">
         <f>#N/A</f>
@@ -4697,8 +4706,11 @@
       <c r="D99" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
       <c r="F99">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G99" t="e">
         <f>#N/A</f>
@@ -4724,8 +4736,11 @@
       <c r="D100" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
       <c r="F100">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4747,8 +4762,11 @@
       <c r="D101" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
       <c r="F101">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G101" t="e">
         <f>#N/A</f>
@@ -4771,8 +4789,11 @@
       <c r="D102" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
       <c r="F102">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G102" t="e">
         <f>#N/A</f>
@@ -4798,8 +4819,11 @@
       <c r="D103" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
       <c r="F103">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4821,8 +4845,11 @@
       <c r="D104" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
       <c r="F104">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G104" t="e">
         <f>#N/A</f>
@@ -4848,8 +4875,11 @@
       <c r="D105" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
       <c r="F105">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4871,8 +4901,11 @@
       <c r="D106" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
       <c r="F106">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G106" t="e">
         <f>#N/A</f>
@@ -4895,8 +4928,11 @@
       <c r="D107" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
       <c r="F107">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G107" t="e">
         <f>#N/A</f>
@@ -4922,8 +4958,11 @@
       <c r="D108" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
       <c r="F108">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -4948,8 +4987,11 @@
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
       <c r="F109">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -5003,8 +5045,11 @@
       <c r="D111" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
       <c r="F111">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -5029,8 +5074,11 @@
       <c r="D112" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
       <c r="F112">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -5052,8 +5100,11 @@
       <c r="D113" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
       <c r="F113">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G113" t="e">
         <f>#N/A</f>
@@ -5160,8 +5211,11 @@
       <c r="D117" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
       <c r="F117">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -5174,7 +5228,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B118" t="s">
@@ -5187,10 +5241,10 @@
         <v>11</v>
       </c>
       <c r="E118">
-        <v>0.43</v>
+        <v>0</v>
       </c>
       <c r="F118">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G118">
         <v>0.43350590239961001</v>
@@ -5215,7 +5269,7 @@
       <c r="D119" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E119" s="4">
+      <c r="E119">
         <v>0.25</v>
       </c>
       <c r="F119">
@@ -5267,8 +5321,11 @@
       <c r="D121" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
       <c r="F121">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G121" t="e">
         <f>#N/A</f>
@@ -5291,8 +5348,11 @@
       <c r="D122" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
       <c r="F122">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G122" t="e">
         <f>#N/A</f>
@@ -5315,8 +5375,11 @@
       <c r="D123" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
       <c r="F123">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G123" t="e">
         <f>#N/A</f>
@@ -5339,8 +5402,11 @@
       <c r="D124" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
       <c r="F124">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G124" t="e">
         <f>#N/A</f>
@@ -5440,8 +5506,11 @@
       <c r="D128" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
       <c r="F128">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G128">
         <v>0</v>
@@ -5463,8 +5532,11 @@
       <c r="D129" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
       <c r="F129">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G129" t="e">
         <f>#N/A</f>
@@ -5487,8 +5559,11 @@
       <c r="D130" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
       <c r="F130">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G130" t="e">
         <f>#N/A</f>
@@ -5511,8 +5586,11 @@
       <c r="D131" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
       <c r="F131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G131" t="e">
         <f>#N/A</f>
@@ -5535,8 +5613,11 @@
       <c r="D132" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
       <c r="F132">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G132" t="e">
         <f>#N/A</f>
@@ -5617,8 +5698,11 @@
       <c r="D135" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
       <c r="F135">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -5643,8 +5727,11 @@
       <c r="D136" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
       <c r="F136">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G136" t="e">
         <f>#N/A</f>
@@ -5658,7 +5745,7 @@
       </c>
     </row>
     <row r="137" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B137" t="s">
@@ -5671,10 +5758,10 @@
         <v>11</v>
       </c>
       <c r="E137">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="F137">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G137">
         <v>0.493984381695803</v>
@@ -5702,8 +5789,11 @@
       <c r="D138" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
       <c r="F138">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G138">
         <v>0</v>
@@ -5734,8 +5824,11 @@
       <c r="D139" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
       <c r="F139">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -5813,8 +5906,11 @@
       <c r="D142" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
       <c r="F142">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G142" t="e">
         <f>#N/A</f>
@@ -5915,7 +6011,7 @@
       </c>
     </row>
     <row r="146" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B146" t="s">
@@ -5928,10 +6024,10 @@
         <v>11</v>
       </c>
       <c r="E146">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="F146">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G146">
         <v>0.57800786986614705</v>
@@ -5956,8 +6052,11 @@
       <c r="D147" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
       <c r="F147">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G147">
         <v>0</v>
@@ -5982,8 +6081,11 @@
       <c r="D148" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
       <c r="F148">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G148">
         <v>0</v>
@@ -6008,8 +6110,11 @@
       <c r="D149" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
       <c r="F149">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G149">
         <v>0</v>
@@ -6034,8 +6139,11 @@
       <c r="D150" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
       <c r="F150">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G150">
         <v>0</v>
@@ -6150,8 +6258,11 @@
       <c r="D154" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
       <c r="F154">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G154">
         <v>0</v>
@@ -6176,8 +6287,11 @@
       <c r="D155" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
       <c r="F155">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G155" t="e">
         <f>#N/A</f>
@@ -6220,7 +6334,7 @@
       </c>
     </row>
     <row r="157" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
+      <c r="A157" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B157" t="s">
@@ -6233,10 +6347,10 @@
         <v>11</v>
       </c>
       <c r="E157">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F157">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G157">
         <v>0.30424992375279603</v>
@@ -6288,8 +6402,11 @@
       <c r="D159" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
       <c r="F159">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G159">
         <v>0</v>
@@ -6311,8 +6428,11 @@
       <c r="D160" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
       <c r="F160">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G160" t="e">
         <f>#N/A</f>
@@ -6338,8 +6458,11 @@
       <c r="D161" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
       <c r="F161">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G161">
         <v>0</v>
@@ -6361,8 +6484,11 @@
       <c r="D162" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
       <c r="F162">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G162" t="e">
         <f>#N/A</f>
@@ -6464,8 +6590,11 @@
       <c r="D166" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E166">
+        <v>0</v>
+      </c>
       <c r="F166">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G166" t="e">
         <f>#N/A</f>
@@ -6518,8 +6647,11 @@
       <c r="D168" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
       <c r="F168">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G168">
         <v>0</v>
@@ -6783,8 +6915,11 @@
       <c r="D177" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
       <c r="F177">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G177">
         <v>0</v>
@@ -6939,7 +7074,7 @@
       </c>
     </row>
     <row r="183" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="4" t="s">
         <v>249</v>
       </c>
       <c r="B183" t="s">
@@ -6952,10 +7087,10 @@
         <v>11</v>
       </c>
       <c r="E183">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="F183">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G183">
         <v>0.43636230347513899</v>
@@ -6983,8 +7118,11 @@
       <c r="D184" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
       <c r="F184">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G184" t="e">
         <f>#N/A</f>
@@ -7071,8 +7209,11 @@
       <c r="D187" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E187">
+        <v>0</v>
+      </c>
       <c r="F187">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G187" t="e">
         <f>#N/A</f>
@@ -7095,8 +7236,11 @@
       <c r="D188" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
       <c r="F188">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G188" t="e">
         <f>#N/A</f>
@@ -7180,8 +7324,11 @@
       <c r="D191" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
       <c r="F191">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G191" t="e">
         <f>#N/A</f>
@@ -7204,8 +7351,11 @@
       <c r="D192" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
       <c r="F192">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G192" t="e">
         <f>#N/A</f>

</xml_diff>